<commit_message>
Make test data less normalized
</commit_message>
<xml_diff>
--- a/files/not_normalized.xlsx
+++ b/files/not_normalized.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t xml:space="preserve">Meine Produktionsdaten</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">Nein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kommentar zu dieser Messung</t>
   </si>
   <si>
     <t xml:space="preserve">2019-03-06 10:52:35</t>
@@ -100,6 +103,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -121,6 +125,7 @@
       <sz val="18"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -170,7 +175,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -203,17 +208,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:H13"/>
+  <dimension ref="A2:J13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+      <selection pane="topLeft" activeCell="J7" activeCellId="0" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -294,10 +299,13 @@
       <c r="G6" s="0" t="s">
         <v>13</v>
       </c>
+      <c r="J6" s="0" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
@@ -321,7 +329,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>9</v>
@@ -347,7 +355,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>6</v>
@@ -370,7 +378,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>7</v>
@@ -390,7 +398,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>2</v>
@@ -416,7 +424,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>10</v>
@@ -439,7 +447,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>7</v>

</xml_diff>